<commit_message>
setting up schema and db and apiroutes
</commit_message>
<xml_diff>
--- a/Master Car List.xlsx
+++ b/Master Car List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Master Car Park\Car Wash Share\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rootm\dev\uwbc\uw-sea-fsf-pt-03-2020-u-c\metroApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0563CCA-BC86-4267-B984-8AD2F7059A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135"/>
+    <workbookView xWindow="996" yWindow="816" windowWidth="21600" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="204">
   <si>
     <t>130598</t>
   </si>
@@ -573,9 +574,6 @@
   </si>
   <si>
     <t>Space</t>
-  </si>
-  <si>
-    <t>Rentals</t>
   </si>
   <si>
     <t>Car #</t>
@@ -644,7 +642,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -970,1244 +968,720 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="4" max="4" width="11.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="2">
-        <v>216</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="2">
-        <v>817</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="2">
-        <v>407</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="2">
-        <v>713</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="2">
-        <v>715</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B7" s="2">
         <v>317</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="2">
-        <v>813</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2">
         <v>305</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>213</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="2">
-        <v>811</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="2">
-        <v>512</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>4118</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" s="2">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="2">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="2">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="2">
         <v>408</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="2">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="2">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B17" s="2">
         <v>509</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="2">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="2">
         <v>315</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B19" s="2">
         <v>306</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B20" s="2">
         <v>410</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1901</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B21" s="2">
         <v>819</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="2">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B22" s="2">
         <v>411</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B23" s="2">
         <v>809</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="2">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B24" s="2">
         <v>707</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B25" s="2">
         <v>814</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="2">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="2">
         <v>401</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B27" s="2">
         <v>206</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="2">
-        <v>4107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="2">
         <v>402</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E28" s="2">
-        <v>4112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="2">
         <v>4110</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="2">
-        <v>4114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B30" s="2">
         <v>508</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="2">
         <v>103</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E31" s="2">
-        <v>4103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="2">
         <v>205</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E32" s="2">
-        <v>4105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="2">
         <v>1914</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="2">
-        <v>4101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B34" s="2">
         <v>104</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="2">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="2">
         <v>303</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="2">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="2">
         <v>1912</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="2">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="2">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B38" s="2">
         <v>810</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B39" s="2">
         <v>708</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E39" s="2">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B40" s="2">
         <v>815</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E40" s="2">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B41" s="2">
         <v>805</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="2">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B42" s="2">
         <v>505</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E42" s="2">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="2">
         <v>217</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="2">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B44" s="2">
         <v>704</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="2">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="2">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B46" s="2">
         <v>808</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1907</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" s="2">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B48" s="2">
         <v>711</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="2">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="2">
         <v>503</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E49" s="2">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="2">
         <v>404</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="2">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B51" s="2">
         <v>105</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E51" s="2">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B53" s="2">
         <v>716</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="2">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="2">
         <v>308</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E54" s="2">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B55" s="2">
         <v>807</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E55" s="2">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B56" s="2">
         <v>102</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="2">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B57" s="2">
         <v>608</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="2">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B58" s="2">
         <v>310</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E58" s="2">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B59" s="2">
         <v>812</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E59" s="2">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B60" s="2">
         <v>316</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E60" s="2">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B61" s="2">
         <v>116</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61" s="2">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B62" s="2">
         <v>302</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" s="2">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B63" s="2">
         <v>110</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="2">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B64" s="2">
         <v>818</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E64" s="2">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B65" s="2">
         <v>709</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E65" s="2">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B66" s="2">
         <v>213</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E66" s="2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B67" s="2">
         <v>202</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E67" s="2">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B68" s="2">
         <v>710</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B69" s="2">
         <v>211</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E69" s="2">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B70" s="2">
         <v>706</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E70" s="2">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E71" s="2">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B72" s="2">
         <v>806</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E72" s="2">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B73" s="2">
         <v>504</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E73" s="2">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B74" s="2">
         <v>604</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E74" s="2">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B75" s="2">
         <v>109</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E75" s="2">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B76" s="2">
         <v>413</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E76" s="2">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B77" s="2">
         <v>301</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E77" s="2">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B78" s="2">
         <v>705</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E78" s="2">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B79" s="2">
         <v>712</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E79" s="2">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B80" s="2">
         <v>614</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E80" s="2">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E81" s="2">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E83" s="2">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E84" s="2">
-        <v>1903</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>144</v>
       </c>
@@ -2215,7 +1689,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>145</v>
       </c>
@@ -2223,7 +1697,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>47</v>
       </c>
@@ -2231,7 +1705,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>48</v>
       </c>
@@ -2239,7 +1713,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>49</v>
       </c>
@@ -2247,8 +1721,717 @@
         <v>115</v>
       </c>
     </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B93" s="2">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94" s="2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B95" s="2">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B96" s="2">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B97" s="2">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" s="2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B99" s="2">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B100" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B102" s="2">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B103" s="2">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B104" s="2">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B105" s="2">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B106" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B107" s="2">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B108" s="2">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109" s="2">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B110" s="2">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B111" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B113" s="2">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B115" s="2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B116" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B117" s="2">
+        <v>4107</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B118" s="2">
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B119" s="2">
+        <v>4114</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B121" s="2">
+        <v>4103</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B122" s="2">
+        <v>4105</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B123" s="2">
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B124" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B125" s="2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B126" s="2">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B127" s="2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B128" s="2">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B129" s="2">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B130" s="2">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B131" s="2">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B132" s="2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B133" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B134" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B135" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B136" s="2">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B137" s="2">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B138" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B139" s="2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B140" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B141" s="2">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B143" s="2">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B144" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B145" s="2">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B147" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B148" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B149" s="2">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B150" s="2">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B151" s="2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B152" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B153" s="2">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B154" s="2">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B155" s="2">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B156" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B157" s="2">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B159" s="2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B160" s="2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B161" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B162" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B163" s="2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B164" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B165" s="2">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B166" s="2">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B167" s="2">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B168" s="2">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B169" s="2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B170" s="2">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B171" s="2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B173" s="2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B174" s="2">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="F1:F183">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F1:F183">
     <sortCondition ref="F85"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>